<commit_message>
Author         : PriyankaChaudhary Files modified : PriyankaChaudhary.xlsx Description    : Task Breakdown with Time estimation
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PriyankaChaudhary.xlsx
+++ b/TeamDetails/TasksBreakDown/PriyankaChaudhary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Priyanka Chaudhary\Desktop\SmaltandBeryl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internship_2017_Prep.git\trunk\TeamDetails\TasksBreakDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -99,12 +99,6 @@
     <t>Block diagram of entire code journey</t>
   </si>
   <si>
-    <t>Save the SignUp page data in the Scope of angular js controller</t>
-  </si>
-  <si>
-    <t>Use this scope in Profile Creation page to show the data entered in SignUp page</t>
-  </si>
-  <si>
     <t>Technical workflow Understanding</t>
   </si>
   <si>
@@ -118,12 +112,18 @@
     <t xml:space="preserve">
 Save the data of Sign-up page in the database, after validating from database </t>
   </si>
+  <si>
+    <t>Get the SignUp page data from the backend</t>
+  </si>
+  <si>
+    <t>Populate that data on the Profile Creation page to show the data entered in SignUp page</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,13 +135,6 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -243,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -262,16 +255,10 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -285,27 +272,42 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2889,7 +2891,7 @@
   <dimension ref="A2:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E14"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2904,7 +2906,7 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>6</v>
@@ -2926,171 +2928,202 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="6"/>
+      <c r="A3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="21">
+        <v>20</v>
+      </c>
       <c r="C3" s="7">
         <v>1</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
       <c r="G3" s="6">
         <f>E3-F3</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="7">
         <v>2</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
       <c r="G4" s="6">
-        <f t="shared" ref="G4:G48" si="0">E4-F4</f>
+        <f t="shared" ref="G4:G27" si="0">E4-F4</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="6"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="7">
         <v>3</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="E5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="6">
+        <f>E5-F5</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="19"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="7">
         <v>4</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="20"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="7">
         <v>5</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="6">
+        <v>1</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="20"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="7">
         <v>6</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="6"/>
+      <c r="E8" s="6">
+        <v>1</v>
+      </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="20"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="7">
         <v>7</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="6">
+        <v>1</v>
+      </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="20"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="7">
         <v>8</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="6">
+        <v>2</v>
+      </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="20"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="7">
         <v>9</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="6"/>
+      <c r="E11" s="6">
+        <v>2</v>
+      </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="20"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="7">
         <v>10</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="23"/>
+      <c r="E12" s="22">
+        <v>6</v>
+      </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="20"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="7">
         <v>11</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="24"/>
+      <c r="E13" s="23"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6">
         <f t="shared" si="0"/>
@@ -3098,15 +3131,15 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="10">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="9">
         <v>12</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="25"/>
+      <c r="E14" s="24"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6">
         <f t="shared" si="0"/>
@@ -3114,213 +3147,241 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="6"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="7">
         <v>13</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="6"/>
+      <c r="E15" s="6">
+        <v>1</v>
+      </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="7">
         <v>14</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="6"/>
+      <c r="E16" s="6">
+        <v>1</v>
+      </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="7">
         <v>15</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="6"/>
+      <c r="E17" s="6">
+        <v>1</v>
+      </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="6"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="7">
         <v>16</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="6"/>
+      <c r="E18" s="6">
+        <v>0.5</v>
+      </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="25">
+        <v>10</v>
+      </c>
+      <c r="C19" s="13">
+        <v>1</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="12">
+        <v>1</v>
+      </c>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="13">
+        <v>2</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="12">
+        <v>1</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="13">
+        <v>3</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="13">
+        <v>4</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15">
+      <c r="E22" s="12">
         <v>1</v>
       </c>
-      <c r="D19" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15">
+      <c r="F22" s="12"/>
+      <c r="G22" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="13">
+        <v>5</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="26">
         <v>2</v>
       </c>
-      <c r="D20" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15">
-        <v>3</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15">
-        <v>4</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15">
-        <v>5</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="13">
         <v>6</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="E24" s="12">
+        <v>1</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15">
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="13">
         <v>7</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="E25" s="12">
+        <v>1</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15">
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="13">
         <v>8</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="E26" s="12">
+        <v>1</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15">
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="13">
         <v>9</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="E27" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -3331,7 +3392,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G4:G48" si="1">E28-F28</f>
         <v>0</v>
       </c>
     </row>
@@ -3343,7 +3404,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3355,21 +3416,21 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="12"/>
+      <c r="C31" s="10"/>
       <c r="D31" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3381,7 +3442,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3393,7 +3454,7 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3405,7 +3466,7 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3417,7 +3478,7 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3429,7 +3490,7 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3441,7 +3502,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3453,7 +3514,7 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3465,7 +3526,7 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3477,7 +3538,7 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3489,7 +3550,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3501,7 +3562,7 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3513,7 +3574,7 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3525,7 +3586,7 @@
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3537,7 +3598,7 @@
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3549,7 +3610,7 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3561,7 +3622,7 @@
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3573,15 +3634,17 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A3:A18"/>
     <mergeCell ref="A19:A27"/>
     <mergeCell ref="E12:E14"/>
+    <mergeCell ref="B3:B18"/>
+    <mergeCell ref="B19:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author         : PriyankaChaudhary Files modified : PriyankaChaudhary.xlsx Description    : MOdification in Task Breakdown with Time estimation
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PriyankaChaudhary.xlsx
+++ b/TeamDetails/TasksBreakDown/PriyankaChaudhary.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
   <si>
     <t>Story ID</t>
   </si>
@@ -118,12 +118,18 @@
   <si>
     <t>Populate that data on the Profile Creation page to show the data entered in SignUp page</t>
   </si>
+  <si>
+    <t>POPULATE THE SIGN-UP DATA on PROFILE CREATION PAGE</t>
+  </si>
+  <si>
+    <t>SAVE THE DATA IN THE DATABASE AFTER VALIDATING THE EXISTENCE OF USER</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,8 +145,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,8 +185,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -232,11 +258,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -272,6 +335,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -291,9 +360,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -302,11 +368,39 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2888,10 +2982,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G48"/>
+  <dimension ref="A2:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2928,37 +3022,28 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="33"/>
+      <c r="B3" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="35"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B4" s="26">
         <v>20</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C4" s="7">
         <v>1</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="E3" s="6">
-        <v>1</v>
-      </c>
-      <c r="F3" s="6">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6">
-        <f>E3-F3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="7">
-        <v>2</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="E4" s="6">
         <v>1</v>
@@ -2967,71 +3052,73 @@
         <v>1</v>
       </c>
       <c r="G4" s="6">
-        <f t="shared" ref="G4:G27" si="0">E4-F4</f>
+        <f>E4-F4</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="7">
+        <v>2</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6">
+        <f t="shared" ref="G5:G29" si="0">E5-F5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="7">
         <v>3</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E6" s="6">
         <v>0.5</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F6" s="6">
         <v>0.5</v>
       </c>
-      <c r="G5" s="6">
-        <f>E5-F5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="7">
+      <c r="G6" s="6">
+        <f>E6-F6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="7">
         <v>4</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>7</v>
-      </c>
-      <c r="E6" s="6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="7">
-        <v>5</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>8</v>
       </c>
       <c r="E7" s="6">
         <v>1</v>
       </c>
       <c r="F7" s="6"/>
-      <c r="G7" s="6">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E8" s="6">
         <v>1</v>
@@ -3043,13 +3130,13 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="6">
         <v>1</v>
@@ -3061,31 +3148,31 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E10" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="7">
+        <v>8</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>9</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>10</v>
       </c>
       <c r="E11" s="6">
         <v>2</v>
@@ -3096,48 +3183,50 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="7">
+        <v>9</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="22">
-        <v>6</v>
+      <c r="E12" s="6">
+        <v>2</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6">
         <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="7">
+        <v>10</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="23">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="7">
-        <v>11</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="23"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="7">
+        <v>11</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>12</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>13</v>
       </c>
       <c r="E14" s="24"/>
       <c r="F14" s="6"/>
@@ -3147,31 +3236,29 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="7">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="9">
+        <v>12</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="6">
-        <v>1</v>
-      </c>
+      <c r="E15" s="25"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="7">
+        <v>13</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>15</v>
       </c>
       <c r="E16" s="6">
         <v>1</v>
@@ -3183,13 +3270,13 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="7">
+        <v>14</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="E17" s="6">
         <v>1</v>
@@ -3201,89 +3288,82 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="16"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
       <c r="C18" s="7">
+        <v>15</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>19</v>
-      </c>
       <c r="E18" s="6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="28">
+        <v>16</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="30">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+      <c r="F19" s="30"/>
+      <c r="G19" s="30">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="32"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="25">
+      <c r="B21" s="27">
         <v>10</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C21" s="13">
         <v>1</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D21" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E21" s="12">
         <v>1</v>
-      </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="13">
-        <v>2</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="12">
-        <v>1</v>
-      </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="13">
-        <v>3</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="12">
-        <v>0.5</v>
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="12">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
       <c r="C22" s="13">
-        <v>4</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>27</v>
+        <v>2</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="E22" s="12">
         <v>1</v>
@@ -3294,32 +3374,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
       <c r="C23" s="13">
-        <v>5</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="26">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="12">
+        <v>0.5</v>
       </c>
       <c r="F23" s="12"/>
       <c r="G23" s="12">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
       <c r="C24" s="13">
-        <v>6</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>14</v>
+        <v>4</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>27</v>
       </c>
       <c r="E24" s="12">
         <v>1</v>
@@ -3330,32 +3410,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
       <c r="C25" s="13">
-        <v>7</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="12">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="16">
+        <v>2</v>
       </c>
       <c r="F25" s="12"/>
       <c r="G25" s="12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
       <c r="C26" s="13">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E26" s="12">
         <v>1</v>
@@ -3367,45 +3447,57 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="13">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E27" s="12">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="12">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="13">
+        <v>8</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="12">
+        <v>1</v>
+      </c>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="22"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="13">
+        <v>9</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="12">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2">
-        <f t="shared" ref="G4:G48" si="1">E28-F28</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -3416,17 +3508,15 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G30:G50" si="1">E30-F30</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="3"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2">
@@ -3449,8 +3539,10 @@
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="3"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2">
@@ -3638,13 +3730,39 @@
         <v>0</v>
       </c>
     </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A3:A18"/>
-    <mergeCell ref="A19:A27"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="B3:B18"/>
-    <mergeCell ref="B19:B27"/>
+  <mergeCells count="7">
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="A4:A19"/>
+    <mergeCell ref="A21:A29"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="B4:B19"/>
+    <mergeCell ref="B21:B29"/>
+    <mergeCell ref="B20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author               : Priyanka Chaudhary Task                 : Track the hours burnt to implement the story assigned in sprint-2 Files modified       : PriyankaChaudhary.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PriyankaChaudhary.xlsx
+++ b/TeamDetails/TasksBreakDown/PriyankaChaudhary.xlsx
@@ -299,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -341,6 +341,28 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -360,46 +382,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2984,8 +2978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:G20"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3022,21 +3016,21 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="36" t="s">
+      <c r="A3" s="20"/>
+      <c r="B3" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="24"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="31">
         <v>20</v>
       </c>
       <c r="C4" s="7">
@@ -3057,8 +3051,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="7">
         <v>2</v>
       </c>
@@ -3077,8 +3071,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
       <c r="C6" s="7">
         <v>3</v>
       </c>
@@ -3097,8 +3091,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="7">
         <v>4</v>
       </c>
@@ -3108,12 +3102,14 @@
       <c r="E7" s="6">
         <v>1</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="7">
         <v>5</v>
       </c>
@@ -3123,15 +3119,17 @@
       <c r="E8" s="6">
         <v>1</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="6">
+        <v>1</v>
+      </c>
       <c r="G8" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="7">
         <v>6</v>
       </c>
@@ -3148,8 +3146,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="7">
         <v>7</v>
       </c>
@@ -3159,15 +3157,17 @@
       <c r="E10" s="6">
         <v>1</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
       <c r="G10" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
       <c r="C11" s="7">
         <v>8</v>
       </c>
@@ -3184,8 +3184,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
       <c r="C12" s="7">
         <v>9</v>
       </c>
@@ -3195,65 +3195,75 @@
       <c r="E12" s="6">
         <v>2</v>
       </c>
-      <c r="F12" s="6"/>
+      <c r="F12" s="6">
+        <v>1</v>
+      </c>
       <c r="G12" s="6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="7">
         <v>10</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="23">
-        <v>6</v>
-      </c>
-      <c r="F13" s="6"/>
+      <c r="E13" s="21">
+        <v>2</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1</v>
+      </c>
       <c r="G13" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="7">
         <v>11</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="6"/>
+      <c r="E14" s="21">
+        <v>2</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1</v>
+      </c>
       <c r="G14" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
       <c r="C15" s="9">
         <v>12</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="25"/>
+      <c r="E15" s="21">
+        <v>1</v>
+      </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="7">
         <v>13</v>
       </c>
@@ -3270,8 +3280,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="7">
         <v>14</v>
       </c>
@@ -3288,8 +3298,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="7">
         <v>15</v>
       </c>
@@ -3306,39 +3316,39 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="28">
+      <c r="A19" s="27"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="17">
         <v>16</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="19">
         <v>0.5</v>
       </c>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30">
+      <c r="F19" s="19"/>
+      <c r="G19" s="19">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="32"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="35"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="27">
+      <c r="B21" s="32">
         <v>10</v>
       </c>
       <c r="C21" s="13">
@@ -3357,8 +3367,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
       <c r="C22" s="13">
         <v>2</v>
       </c>
@@ -3375,8 +3385,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="21"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
       <c r="C23" s="13">
         <v>3</v>
       </c>
@@ -3393,8 +3403,8 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
       <c r="C24" s="13">
         <v>4</v>
       </c>
@@ -3411,8 +3421,8 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="21"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="13">
         <v>5</v>
       </c>
@@ -3429,8 +3439,8 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
       <c r="C26" s="13">
         <v>6</v>
       </c>
@@ -3447,8 +3457,8 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
-      <c r="B27" s="21"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="13">
         <v>7</v>
       </c>
@@ -3465,8 +3475,8 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="21"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
       <c r="C28" s="13">
         <v>8</v>
       </c>
@@ -3483,8 +3493,8 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="30"/>
       <c r="C29" s="13">
         <v>9</v>
       </c>
@@ -3755,11 +3765,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="A4:A19"/>
     <mergeCell ref="A21:A29"/>
-    <mergeCell ref="E13:E15"/>
     <mergeCell ref="B4:B19"/>
     <mergeCell ref="B21:B29"/>
     <mergeCell ref="B20:G20"/>

</xml_diff>

<commit_message>
Author               : Priyanka Chaudhary Task                 : Add the Remaining hour column and status of each task of the respective stories of sprint:2 Files modified       : PriyankaChaudhary.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PriyankaChaudhary.xlsx
+++ b/TeamDetails/TasksBreakDown/PriyankaChaudhary.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
   <si>
     <t>Story ID</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Block diagram of entire code journey</t>
   </si>
   <si>
-    <t>Technical workflow Understanding</t>
-  </si>
-  <si>
     <t>Story</t>
   </si>
   <si>
@@ -126,6 +123,16 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>HOURS LEFT</t>
+  </si>
+  <si>
+    <t>Remaining</t>
+  </si>
+  <si>
+    <t>Not
+Started</t>
   </si>
 </sst>
 </file>
@@ -157,7 +164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,13 +197,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -327,7 +352,6 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -338,9 +362,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -357,14 +378,72 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -390,17 +469,20 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2982,10 +3064,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H50"/>
+  <dimension ref="A2:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2996,48 +3078,50 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="24"/>
+      <c r="A3" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="57"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="31">
-        <v>20</v>
+      <c r="A4" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="51">
+        <v>19</v>
       </c>
       <c r="C4" s="7">
         <v>1</v>
@@ -3055,10 +3139,13 @@
         <f>E4-F4</f>
         <v>0</v>
       </c>
+      <c r="H4" s="33" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="46"/>
       <c r="C5" s="7">
         <v>2</v>
       </c>
@@ -3072,13 +3159,14 @@
         <v>1</v>
       </c>
       <c r="G5" s="6">
-        <f t="shared" ref="G5:G29" si="0">E5-F5</f>
-        <v>0</v>
-      </c>
+        <f t="shared" ref="G5:G30" si="0">E5-F5</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="46"/>
       <c r="C6" s="7">
         <v>3</v>
       </c>
@@ -3095,14 +3183,15 @@
         <f>E6-F6</f>
         <v>0</v>
       </c>
+      <c r="H6" s="34"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="46"/>
+      <c r="B7" s="46"/>
       <c r="C7" s="7">
         <v>4</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="6">
@@ -3111,15 +3200,19 @@
       <c r="F7" s="6">
         <v>1</v>
       </c>
-      <c r="G7" s="6"/>
+      <c r="G7" s="6">
+        <f>E7-F7</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="34"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="46"/>
       <c r="C8" s="7">
         <v>5</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="6">
@@ -3132,14 +3225,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="H8" s="34"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
+      <c r="A9" s="46"/>
+      <c r="B9" s="46"/>
       <c r="C9" s="7">
         <v>6</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="6">
@@ -3152,14 +3246,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="H9" s="34"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="46"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="7">
         <v>7</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="6">
@@ -3172,14 +3267,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="H10" s="34"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
+      <c r="A11" s="46"/>
+      <c r="B11" s="46"/>
       <c r="C11" s="7">
         <v>8</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="6">
@@ -3192,14 +3288,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="H11" s="34"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="46"/>
       <c r="C12" s="7">
         <v>9</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="6">
@@ -3212,37 +3309,39 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="H12" s="34"/>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
+      <c r="A13" s="46"/>
+      <c r="B13" s="46"/>
       <c r="C13" s="7">
         <v>10</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="36">
+      <c r="E13" s="20">
         <v>2</v>
       </c>
-      <c r="F13" s="36">
+      <c r="F13" s="20">
         <v>1</v>
       </c>
       <c r="G13" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="H13" s="34"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
+      <c r="A14" s="46"/>
+      <c r="B14" s="46"/>
       <c r="C14" s="7">
         <v>11</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="36">
+      <c r="E14" s="20">
         <v>2</v>
       </c>
       <c r="F14" s="6">
@@ -3252,33 +3351,32 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="H14" t="s">
-        <v>31</v>
-      </c>
+      <c r="H14" s="34"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
+      <c r="A15" s="46"/>
+      <c r="B15" s="46"/>
       <c r="C15" s="9">
         <v>12</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="21">
-        <v>1</v>
-      </c>
-      <c r="F15" s="36">
+      <c r="E15" s="19">
+        <v>1</v>
+      </c>
+      <c r="F15" s="20">
         <v>1</v>
       </c>
       <c r="G15" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="H15" s="35"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="46"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="7">
         <v>13</v>
       </c>
@@ -3289,16 +3387,19 @@
         <v>1</v>
       </c>
       <c r="F16" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+        <v>1</v>
+      </c>
+      <c r="H16" s="36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="46"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="7">
         <v>14</v>
       </c>
@@ -3313,10 +3414,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
+      <c r="H17" s="37"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="46"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="7">
         <v>15</v>
       </c>
@@ -3331,263 +3433,271 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="17">
+      <c r="H18" s="37"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="47"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="15">
         <v>16</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="17">
         <v>0.5</v>
       </c>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19">
+      <c r="F19" s="17"/>
+      <c r="G19" s="17">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="35"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="32">
-        <v>10</v>
-      </c>
-      <c r="C21" s="13">
-        <v>1</v>
-      </c>
-      <c r="D21" s="14" t="s">
+      <c r="H19" s="38"/>
+    </row>
+    <row r="20" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="21"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="54"/>
+      <c r="G20" s="26">
+        <f>SUM(G4:G19)</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="44"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="52">
+        <v>9</v>
+      </c>
+      <c r="C22" s="12">
+        <v>1</v>
+      </c>
+      <c r="D22" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="12">
-        <v>1</v>
-      </c>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="13">
+      <c r="E22" s="11">
+        <v>1</v>
+      </c>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H22" s="39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="49"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="12">
         <v>2</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D23" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="12">
-        <v>1</v>
-      </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="13">
+      <c r="E23" s="11">
+        <v>1</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H23" s="40"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="49"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="12">
         <v>3</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D24" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E24" s="11">
         <v>0.5</v>
       </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12">
+      <c r="F24" s="11"/>
+      <c r="G24" s="11">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="13">
+      <c r="H24" s="40"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="49"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="12">
         <v>4</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D25" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="11">
+        <v>1</v>
+      </c>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H25" s="40"/>
+    </row>
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="49"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="12">
+        <v>5</v>
+      </c>
+      <c r="D26" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="12">
-        <v>1</v>
-      </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="13">
-        <v>5</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="16">
+      <c r="E26" s="14">
         <v>2</v>
       </c>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12">
+      <c r="F26" s="11"/>
+      <c r="G26" s="11">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="13">
+      <c r="H26" s="40"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="49"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="12">
         <v>6</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D27" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="12">
-        <v>1</v>
-      </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="13">
+      <c r="E27" s="11">
+        <v>1</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H27" s="40"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="49"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="12">
         <v>7</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D28" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="12">
-        <v>1</v>
-      </c>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="13">
+      <c r="E28" s="11">
+        <v>1</v>
+      </c>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H28" s="40"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="49"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="12">
         <v>8</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D29" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="12">
-        <v>1</v>
-      </c>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="13">
+      <c r="E29" s="11">
+        <v>1</v>
+      </c>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H29" s="40"/>
+      <c r="I29" s="28"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="50"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="12">
         <v>9</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D30" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="12">
+      <c r="E30" s="11">
         <v>0.5</v>
       </c>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12">
+      <c r="F30" s="11"/>
+      <c r="G30" s="11">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2">
-        <f t="shared" ref="G30:G50" si="1">E30-F30</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="41"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E31" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="32"/>
+      <c r="G31" s="27">
+        <f>SUM(G22:G30)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="3"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="G32" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="3"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
-      <c r="G33" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+      <c r="C34" s="30"/>
       <c r="D34" s="3"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
@@ -3596,10 +3706,7 @@
       <c r="D35" s="3"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
-      <c r="G35" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G35" s="2"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
@@ -3608,10 +3715,7 @@
       <c r="D36" s="3"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
@@ -3620,10 +3724,7 @@
       <c r="D37" s="3"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G37" s="2"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
@@ -3632,10 +3733,7 @@
       <c r="D38" s="3"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G38" s="2"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
@@ -3644,10 +3742,7 @@
       <c r="D39" s="3"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G39" s="2"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
@@ -3656,10 +3751,7 @@
       <c r="D40" s="3"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
-      <c r="G40" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
@@ -3668,10 +3760,7 @@
       <c r="D41" s="3"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G41" s="2"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
@@ -3680,10 +3769,7 @@
       <c r="D42" s="3"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G42" s="2"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
@@ -3692,10 +3778,7 @@
       <c r="D43" s="3"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
-      <c r="G43" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G43" s="2"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
@@ -3704,10 +3787,7 @@
       <c r="D44" s="3"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
-      <c r="G44" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G44" s="2"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
@@ -3716,10 +3796,7 @@
       <c r="D45" s="3"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
-      <c r="G45" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G45" s="2"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
@@ -3728,10 +3805,7 @@
       <c r="D46" s="3"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-      <c r="G46" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G46" s="2"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
@@ -3740,10 +3814,7 @@
       <c r="D47" s="3"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
-      <c r="G47" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G47" s="2"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
@@ -3752,10 +3823,7 @@
       <c r="D48" s="3"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
-      <c r="G48" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G48" s="2"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
@@ -3764,10 +3832,7 @@
       <c r="D49" s="3"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
-      <c r="G49" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G49" s="2"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
@@ -3776,19 +3841,30 @@
       <c r="D50" s="3"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
-      <c r="G50" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B3:G3"/>
+  <mergeCells count="11">
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="H4:H15"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="H22:H30"/>
+    <mergeCell ref="A21:H21"/>
     <mergeCell ref="A4:A19"/>
-    <mergeCell ref="A21:A29"/>
+    <mergeCell ref="A22:A30"/>
     <mergeCell ref="B4:B19"/>
-    <mergeCell ref="B21:B29"/>
-    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B22:B30"/>
+    <mergeCell ref="E20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author               : Priyanka Chaudhary Task                 : Updating the status of each task of the respective stories of sprint:2 Files modified       : PriyankaChaudhary.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PriyankaChaudhary.xlsx
+++ b/TeamDetails/TasksBreakDown/PriyankaChaudhary.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
   <si>
     <t>Story ID</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Establish the JDBC connection</t>
   </si>
   <si>
-    <t>SVN Commit</t>
-  </si>
-  <si>
     <t>Understanding the why of the story</t>
   </si>
   <si>
@@ -131,8 +128,10 @@
     <t>Remaining</t>
   </si>
   <si>
-    <t>Not
-Started</t>
+    <t>Unit Testing and error fixing</t>
+  </si>
+  <si>
+    <t>Not Started</t>
   </si>
 </sst>
 </file>
@@ -226,7 +225,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -323,11 +322,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -381,6 +391,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -396,6 +409,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -415,21 +434,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -454,9 +458,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -466,9 +467,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -484,6 +482,24 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3066,8 +3082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B19"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3083,7 +3099,7 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>6</v>
@@ -3091,7 +3107,7 @@
       <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="32" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="18" t="s">
@@ -3105,29 +3121,29 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="57"/>
+      <c r="A3" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="53"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="51">
+      <c r="A4" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="48">
         <v>19</v>
       </c>
       <c r="C4" s="7">
         <v>1</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="6">
         <v>1</v>
@@ -3139,18 +3155,18 @@
         <f>E4-F4</f>
         <v>0</v>
       </c>
-      <c r="H4" s="33" t="s">
-        <v>30</v>
+      <c r="H4" s="36" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
-      <c r="B5" s="46"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="7">
         <v>2</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="6">
         <v>1</v>
@@ -3162,16 +3178,16 @@
         <f t="shared" ref="G5:G30" si="0">E5-F5</f>
         <v>0</v>
       </c>
-      <c r="H5" s="34"/>
+      <c r="H5" s="37"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="46"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="7">
         <v>3</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="6">
         <v>0.5</v>
@@ -3183,11 +3199,11 @@
         <f>E6-F6</f>
         <v>0</v>
       </c>
-      <c r="H6" s="34"/>
+      <c r="H6" s="37"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="46"/>
+      <c r="A7" s="44"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="7">
         <v>4</v>
       </c>
@@ -3204,11 +3220,11 @@
         <f>E7-F7</f>
         <v>0</v>
       </c>
-      <c r="H7" s="34"/>
+      <c r="H7" s="37"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
-      <c r="B8" s="46"/>
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
       <c r="C8" s="7">
         <v>5</v>
       </c>
@@ -3225,11 +3241,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="34"/>
+      <c r="H8" s="37"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
-      <c r="B9" s="46"/>
+      <c r="A9" s="44"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="7">
         <v>6</v>
       </c>
@@ -3246,11 +3262,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H9" s="34"/>
+      <c r="H9" s="37"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
-      <c r="B10" s="46"/>
+      <c r="A10" s="44"/>
+      <c r="B10" s="44"/>
       <c r="C10" s="7">
         <v>7</v>
       </c>
@@ -3267,11 +3283,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="34"/>
+      <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="46"/>
+      <c r="A11" s="44"/>
+      <c r="B11" s="44"/>
       <c r="C11" s="7">
         <v>8</v>
       </c>
@@ -3288,11 +3304,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="34"/>
+      <c r="H11" s="37"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
-      <c r="B12" s="46"/>
+      <c r="A12" s="44"/>
+      <c r="B12" s="44"/>
       <c r="C12" s="7">
         <v>9</v>
       </c>
@@ -3309,11 +3325,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H12" s="34"/>
+      <c r="H12" s="37"/>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
-      <c r="B13" s="46"/>
+      <c r="A13" s="44"/>
+      <c r="B13" s="44"/>
       <c r="C13" s="7">
         <v>10</v>
       </c>
@@ -3330,11 +3346,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="34"/>
+      <c r="H13" s="37"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
-      <c r="B14" s="46"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="44"/>
       <c r="C14" s="7">
         <v>11</v>
       </c>
@@ -3351,11 +3367,11 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="H14" s="34"/>
+      <c r="H14" s="37"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="46"/>
-      <c r="B15" s="46"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="44"/>
       <c r="C15" s="9">
         <v>12</v>
       </c>
@@ -3372,34 +3388,32 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H15" s="35"/>
+      <c r="H15" s="37"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="46"/>
-      <c r="B16" s="46"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="44"/>
       <c r="C16" s="7">
         <v>13</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="E16" s="6">
         <v>1</v>
       </c>
       <c r="F16" s="6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G16" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H16" s="36" t="s">
-        <v>32</v>
-      </c>
+        <v>-3</v>
+      </c>
+      <c r="H16" s="37"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
       <c r="C17" s="7">
         <v>14</v>
       </c>
@@ -3414,11 +3428,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="37"/>
+      <c r="H17" s="29" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
-      <c r="B18" s="46"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
       <c r="C18" s="7">
         <v>15</v>
       </c>
@@ -3433,124 +3449,115 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H18" s="37"/>
+      <c r="H18" s="30"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
-      <c r="B19" s="46"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="44"/>
       <c r="C19" s="15">
         <v>16</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="54"/>
+    </row>
+    <row r="20" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="50"/>
+      <c r="G20" s="27">
+        <f>SUM(G4:G19)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="42"/>
+    </row>
+    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="46">
+        <v>9</v>
+      </c>
+      <c r="C22" s="21">
+        <v>1</v>
+      </c>
+      <c r="D22" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="H19" s="38"/>
-    </row>
-    <row r="20" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="54"/>
-      <c r="G20" s="26">
-        <f>SUM(G4:G19)</f>
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="44"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="52">
-        <v>9</v>
-      </c>
-      <c r="C22" s="12">
-        <v>1</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="11">
-        <v>1</v>
-      </c>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H22" s="39" t="s">
-        <v>33</v>
-      </c>
+      <c r="E22" s="60">
+        <v>1</v>
+      </c>
+      <c r="F22" s="60"/>
+      <c r="G22" s="61">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H22" s="56"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
-      <c r="B23" s="49"/>
+      <c r="A23" s="46"/>
+      <c r="B23" s="46"/>
       <c r="C23" s="12">
         <v>2</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E23" s="11">
         <v>1</v>
       </c>
       <c r="F23" s="11"/>
-      <c r="G23" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H23" s="40"/>
+      <c r="G23" s="55">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H23" s="57"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
-      <c r="B24" s="49"/>
+      <c r="A24" s="46"/>
+      <c r="B24" s="46"/>
       <c r="C24" s="12">
         <v>3</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E24" s="11">
         <v>0.5</v>
       </c>
       <c r="F24" s="11"/>
-      <c r="G24" s="11">
+      <c r="G24" s="55">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="H24" s="40"/>
+      <c r="H24" s="57"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
-      <c r="B25" s="49"/>
+      <c r="A25" s="46"/>
+      <c r="B25" s="46"/>
       <c r="C25" s="12">
         <v>4</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E25" s="11">
         <v>1</v>
@@ -3560,16 +3567,18 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="40"/>
+      <c r="H25" s="38" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="49"/>
-      <c r="B26" s="49"/>
+      <c r="A26" s="46"/>
+      <c r="B26" s="46"/>
       <c r="C26" s="12">
         <v>5</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E26" s="14">
         <v>2</v>
@@ -3579,11 +3588,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H26" s="40"/>
+      <c r="H26" s="38"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="49"/>
-      <c r="B27" s="49"/>
+      <c r="A27" s="46"/>
+      <c r="B27" s="46"/>
       <c r="C27" s="12">
         <v>6</v>
       </c>
@@ -3598,11 +3607,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="40"/>
+      <c r="H27" s="38"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="49"/>
-      <c r="B28" s="49"/>
+      <c r="A28" s="46"/>
+      <c r="B28" s="46"/>
       <c r="C28" s="12">
         <v>7</v>
       </c>
@@ -3617,11 +3626,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H28" s="40"/>
+      <c r="H28" s="38"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="49"/>
-      <c r="B29" s="49"/>
+      <c r="A29" s="46"/>
+      <c r="B29" s="46"/>
       <c r="C29" s="12">
         <v>8</v>
       </c>
@@ -3636,40 +3645,33 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H29" s="40"/>
-      <c r="I29" s="28"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="31"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="50"/>
-      <c r="B30" s="50"/>
+      <c r="A30" s="47"/>
+      <c r="B30" s="47"/>
       <c r="C30" s="12">
         <v>9</v>
       </c>
-      <c r="D30" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E30" s="11">
-        <v>0.5</v>
-      </c>
+      <c r="D30" s="13"/>
+      <c r="E30" s="11"/>
       <c r="F30" s="11"/>
-      <c r="G30" s="11">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="H30" s="41"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="39"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="F31" s="32"/>
-      <c r="G31" s="27">
+      <c r="E31" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" s="35"/>
+      <c r="G31" s="28">
         <f>SUM(G22:G30)</f>
-        <v>9</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -3693,7 +3695,7 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="30"/>
+      <c r="C34" s="33"/>
       <c r="D34" s="3"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -3853,12 +3855,11 @@
       <c r="G51" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="10">
     <mergeCell ref="A3:H3"/>
+    <mergeCell ref="H4:H16"/>
+    <mergeCell ref="H25:H30"/>
     <mergeCell ref="E31:F31"/>
-    <mergeCell ref="H4:H15"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="H22:H30"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A4:A19"/>
     <mergeCell ref="A22:A30"/>

</xml_diff>

<commit_message>
Author              : Priyanka Chaudhary Task                : Updating Sprint-2 sheet
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PriyankaChaudhary.xlsx
+++ b/TeamDetails/TasksBreakDown/PriyankaChaudhary.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="33">
   <si>
     <t>Story ID</t>
   </si>
@@ -125,13 +125,10 @@
     <t>HOURS LEFT</t>
   </si>
   <si>
-    <t>Remaining</t>
-  </si>
-  <si>
     <t>Unit Testing and error fixing</t>
   </si>
   <si>
-    <t>Not Started</t>
+    <t>In Dev</t>
   </si>
 </sst>
 </file>
@@ -163,7 +160,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,12 +194,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -337,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -407,14 +398,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -422,23 +407,29 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -458,6 +449,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -467,39 +461,30 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3082,8 +3067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3107,7 +3092,7 @@
       <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="30" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="18" t="s">
@@ -3121,22 +3106,22 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="53"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="48">
+      <c r="B4" s="51">
         <v>19</v>
       </c>
       <c r="C4" s="7">
@@ -3155,13 +3140,13 @@
         <f>E4-F4</f>
         <v>0</v>
       </c>
-      <c r="H4" s="36" t="s">
+      <c r="H4" s="54" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
-      <c r="B5" s="44"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="46"/>
       <c r="C5" s="7">
         <v>2</v>
       </c>
@@ -3175,14 +3160,14 @@
         <v>1</v>
       </c>
       <c r="G5" s="6">
-        <f t="shared" ref="G5:G30" si="0">E5-F5</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="37"/>
+        <f t="shared" ref="G5:G29" si="0">E5-F5</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="55"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
-      <c r="B6" s="44"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="46"/>
       <c r="C6" s="7">
         <v>3</v>
       </c>
@@ -3199,11 +3184,11 @@
         <f>E6-F6</f>
         <v>0</v>
       </c>
-      <c r="H6" s="37"/>
+      <c r="H6" s="55"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="44"/>
+      <c r="A7" s="46"/>
+      <c r="B7" s="46"/>
       <c r="C7" s="7">
         <v>4</v>
       </c>
@@ -3220,11 +3205,11 @@
         <f>E7-F7</f>
         <v>0</v>
       </c>
-      <c r="H7" s="37"/>
+      <c r="H7" s="55"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
-      <c r="B8" s="44"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="46"/>
       <c r="C8" s="7">
         <v>5</v>
       </c>
@@ -3241,11 +3226,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="37"/>
+      <c r="H8" s="55"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="44"/>
+      <c r="A9" s="46"/>
+      <c r="B9" s="46"/>
       <c r="C9" s="7">
         <v>6</v>
       </c>
@@ -3262,11 +3247,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H9" s="37"/>
+      <c r="H9" s="55"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
-      <c r="B10" s="44"/>
+      <c r="A10" s="46"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="7">
         <v>7</v>
       </c>
@@ -3283,11 +3268,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="37"/>
+      <c r="H10" s="55"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="44"/>
+      <c r="A11" s="46"/>
+      <c r="B11" s="46"/>
       <c r="C11" s="7">
         <v>8</v>
       </c>
@@ -3304,11 +3289,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="37"/>
+      <c r="H11" s="55"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
-      <c r="B12" s="44"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="46"/>
       <c r="C12" s="7">
         <v>9</v>
       </c>
@@ -3325,11 +3310,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H12" s="37"/>
+      <c r="H12" s="55"/>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
-      <c r="B13" s="44"/>
+      <c r="A13" s="46"/>
+      <c r="B13" s="46"/>
       <c r="C13" s="7">
         <v>10</v>
       </c>
@@ -3346,11 +3331,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="37"/>
+      <c r="H13" s="55"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
-      <c r="B14" s="44"/>
+      <c r="A14" s="46"/>
+      <c r="B14" s="46"/>
       <c r="C14" s="7">
         <v>11</v>
       </c>
@@ -3367,11 +3352,11 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="H14" s="37"/>
+      <c r="H14" s="55"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
-      <c r="B15" s="44"/>
+      <c r="A15" s="46"/>
+      <c r="B15" s="46"/>
       <c r="C15" s="9">
         <v>12</v>
       </c>
@@ -3388,16 +3373,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H15" s="37"/>
+      <c r="H15" s="55"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
-      <c r="B16" s="44"/>
+      <c r="A16" s="46"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="7">
         <v>13</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="6">
         <v>1</v>
@@ -3409,11 +3394,11 @@
         <f t="shared" si="0"/>
         <v>-3</v>
       </c>
-      <c r="H16" s="37"/>
+      <c r="H16" s="55"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
-      <c r="B17" s="44"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="7">
         <v>14</v>
       </c>
@@ -3428,13 +3413,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="29" t="s">
-        <v>31</v>
-      </c>
+      <c r="H17" s="55"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
-      <c r="B18" s="44"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="7">
         <v>15</v>
       </c>
@@ -3444,77 +3427,81 @@
       <c r="E18" s="6">
         <v>1</v>
       </c>
-      <c r="F18" s="6"/>
+      <c r="F18" s="6">
+        <v>0</v>
+      </c>
       <c r="G18" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H18" s="30"/>
+      <c r="H18" s="56"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="45"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="15">
-        <v>16</v>
-      </c>
+      <c r="A19" s="47"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="15"/>
       <c r="D19" s="16"/>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
-      <c r="H19" s="54"/>
+      <c r="H19" s="32"/>
     </row>
     <row r="20" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="24"/>
       <c r="D20" s="25"/>
-      <c r="E20" s="49" t="s">
+      <c r="E20" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="50"/>
+      <c r="F20" s="53"/>
       <c r="G20" s="27">
         <f>SUM(G4:G19)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="42"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="44"/>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="58" t="s">
+      <c r="A22" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="46">
+      <c r="B22" s="49">
         <v>9</v>
       </c>
       <c r="C22" s="21">
         <v>1</v>
       </c>
-      <c r="D22" s="59" t="s">
+      <c r="D22" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="60">
-        <v>1</v>
-      </c>
-      <c r="F22" s="60"/>
-      <c r="G22" s="61">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H22" s="56"/>
+      <c r="E22" s="35">
+        <v>1</v>
+      </c>
+      <c r="F22" s="35">
+        <v>0</v>
+      </c>
+      <c r="G22" s="36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H22" s="58" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="46"/>
-      <c r="B23" s="46"/>
+      <c r="A23" s="49"/>
+      <c r="B23" s="49"/>
       <c r="C23" s="12">
         <v>2</v>
       </c>
@@ -3524,16 +3511,20 @@
       <c r="E23" s="11">
         <v>1</v>
       </c>
-      <c r="F23" s="11"/>
-      <c r="G23" s="55">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H23" s="57"/>
+      <c r="F23" s="11">
+        <v>0</v>
+      </c>
+      <c r="G23" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H23" s="58" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
-      <c r="B24" s="46"/>
+      <c r="A24" s="49"/>
+      <c r="B24" s="49"/>
       <c r="C24" s="12">
         <v>3</v>
       </c>
@@ -3543,16 +3534,20 @@
       <c r="E24" s="11">
         <v>0.5</v>
       </c>
-      <c r="F24" s="11"/>
-      <c r="G24" s="55">
+      <c r="F24" s="11">
+        <v>0</v>
+      </c>
+      <c r="G24" s="33">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="H24" s="57"/>
+      <c r="H24" s="58" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="46"/>
-      <c r="B25" s="46"/>
+      <c r="A25" s="49"/>
+      <c r="B25" s="49"/>
       <c r="C25" s="12">
         <v>4</v>
       </c>
@@ -3562,18 +3557,20 @@
       <c r="E25" s="11">
         <v>1</v>
       </c>
-      <c r="F25" s="11"/>
+      <c r="F25" s="11">
+        <v>2</v>
+      </c>
       <c r="G25" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H25" s="38" t="s">
-        <v>33</v>
+        <v>-1</v>
+      </c>
+      <c r="H25" s="57" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="46"/>
-      <c r="B26" s="46"/>
+      <c r="A26" s="49"/>
+      <c r="B26" s="49"/>
       <c r="C26" s="12">
         <v>5</v>
       </c>
@@ -3583,16 +3580,20 @@
       <c r="E26" s="14">
         <v>2</v>
       </c>
-      <c r="F26" s="11"/>
+      <c r="F26" s="11">
+        <v>3</v>
+      </c>
       <c r="G26" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H26" s="38"/>
+        <v>-1</v>
+      </c>
+      <c r="H26" s="59" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="46"/>
-      <c r="B27" s="46"/>
+      <c r="A27" s="49"/>
+      <c r="B27" s="49"/>
       <c r="C27" s="12">
         <v>6</v>
       </c>
@@ -3607,11 +3608,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="38"/>
+      <c r="H27" s="57"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="46"/>
-      <c r="B28" s="46"/>
+      <c r="A28" s="49"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="12">
         <v>7</v>
       </c>
@@ -3626,11 +3627,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H28" s="38"/>
+      <c r="H28" s="57"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="46"/>
-      <c r="B29" s="46"/>
+      <c r="A29" s="49"/>
+      <c r="B29" s="49"/>
       <c r="C29" s="12">
         <v>8</v>
       </c>
@@ -3645,12 +3646,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H29" s="38"/>
-      <c r="I29" s="31"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="29"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="47"/>
-      <c r="B30" s="47"/>
+      <c r="A30" s="50"/>
+      <c r="B30" s="50"/>
       <c r="C30" s="12">
         <v>9</v>
       </c>
@@ -3658,20 +3659,20 @@
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
-      <c r="H30" s="39"/>
+      <c r="H30" s="57"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="28">
         <f>SUM(G22:G30)</f>
-        <v>8.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -3695,7 +3696,7 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="33"/>
+      <c r="C34" s="31"/>
       <c r="D34" s="3"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -3855,10 +3856,8 @@
       <c r="G51" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="A3:H3"/>
-    <mergeCell ref="H4:H16"/>
-    <mergeCell ref="H25:H30"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A4:A19"/>
@@ -3866,6 +3865,7 @@
     <mergeCell ref="B4:B19"/>
     <mergeCell ref="B22:B30"/>
     <mergeCell ref="E20:F20"/>
+    <mergeCell ref="H4:H18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>